<commit_message>
notebook to read the excel and create the yaml files'
</commit_message>
<xml_diff>
--- a/files/ETRADE_mov.xlsx
+++ b/files/ETRADE_mov.xlsx
@@ -413,7 +413,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -449,7 +449,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>8</v>

</xml_diff>